<commit_message>
Yooo fam its time to goo now so yeah ehm yeah what we did today is we did add all of the components and somebug fixing yeah that is pretty much all
Good morning today you should do some styling and animating i know you like that but idk if thats so cool but well go through it we dont care if its not cool if it benefit us we going

Also show bernhard what it looks so far and tell em ther is a headset and mouse next to you in the thingy there the schiebewagon-teil-kasten am boden links von dir

oh yeah lastly ma boy you got this stay humble and stay givin you a beast there is no if feel like it consistency my boy consistency, brush your teeth and no going to bed before its done

oh yeah good morning and have a nice day
</commit_message>
<xml_diff>
--- a/src/main/resources/Excel-Files/Estimations.xlsx
+++ b/src/main/resources/Excel-Files/Estimations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lkronlac\Desktop\Data\Project\Frontend\CreatorFrontend\Frontend\src\main\resources\Excel-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD04258D-EFBC-491A-8DA6-2911A1B745F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18844908-F059-48D0-B28F-44026E018FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FBAF2B72-6F99-45BF-BBB2-5ADA9D6D6660}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FBAF2B72-6F99-45BF-BBB2-5ADA9D6D6660}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1760,9 +1760,6 @@
   </si>
   <si>
     <t>MIC-CUST® GUM - Gurantee Management</t>
-  </si>
-  <si>
-    <t>Basic Setup for MIC-INTRA - Instrastat Filing</t>
   </si>
   <si>
     <t>Intrastat Filing</t>
@@ -2058,6 +2055,9 @@
   </si>
   <si>
     <t>MIC_CUST_Stocks_per_Proc__Ctry</t>
+  </si>
+  <si>
+    <t>Basic Setup for MIC-INTRA - Instrastat Filing</t>
   </si>
 </sst>
 </file>
@@ -2589,8 +2589,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:S629"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A299" activePane="bottomLeft" state="frozenSplit"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A461" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="B311" sqref="B311"/>
     </sheetView>
   </sheetViews>
@@ -17871,9 +17871,9 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17899,7 +17899,7 @@
         <v>433</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
@@ -17916,7 +17916,7 @@
         <v>435</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
@@ -17933,7 +17933,7 @@
         <v>438</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="51.6" x14ac:dyDescent="0.3">
@@ -17950,7 +17950,7 @@
         <v>440</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="37.200000000000003" x14ac:dyDescent="0.3">
@@ -17958,7 +17958,7 @@
         <v>88</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>441</v>
@@ -17967,7 +17967,7 @@
         <v>89</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
@@ -17984,7 +17984,7 @@
         <v>443</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="51.6" x14ac:dyDescent="0.3">
@@ -18001,7 +18001,7 @@
         <v>445</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="51.6" x14ac:dyDescent="0.3">
@@ -18018,7 +18018,7 @@
         <v>443</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -18033,7 +18033,7 @@
         <v>448</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
@@ -18050,7 +18050,7 @@
         <v>450</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="54" x14ac:dyDescent="0.3">
@@ -18067,7 +18067,7 @@
         <v>453</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="76.8" x14ac:dyDescent="0.3">
@@ -18084,7 +18084,7 @@
         <v>456</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -18092,14 +18092,14 @@
         <v>144</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C13" s="17"/>
       <c r="D13" s="13" t="s">
         <v>457</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -18114,7 +18114,7 @@
         <v>448</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
@@ -18129,7 +18129,7 @@
         <v>241</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -18144,7 +18144,7 @@
         <v>448</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
@@ -18161,7 +18161,7 @@
         <v>462</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="51.6" x14ac:dyDescent="0.3">
@@ -18178,7 +18178,7 @@
         <v>465</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -18195,7 +18195,7 @@
         <v>468</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="51.6" x14ac:dyDescent="0.3">
@@ -18212,7 +18212,7 @@
         <v>471</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="37.200000000000003" x14ac:dyDescent="0.3">
@@ -18229,7 +18229,7 @@
         <v>348</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -18244,7 +18244,7 @@
         <v>354</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -18258,7 +18258,7 @@
         <v>462</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
@@ -18269,13 +18269,13 @@
         <v>20</v>
       </c>
       <c r="C24" s="16" t="s">
+        <v>548</v>
+      </c>
+      <c r="D24" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="D24" s="13" t="s">
-        <v>476</v>
-      </c>
       <c r="E24" s="13" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="36.6" x14ac:dyDescent="0.3">
@@ -18283,16 +18283,16 @@
         <v>374</v>
       </c>
       <c r="B25" s="13" t="s">
+        <v>476</v>
+      </c>
+      <c r="C25" s="16" t="s">
         <v>477</v>
       </c>
-      <c r="C25" s="16" t="s">
-        <v>478</v>
-      </c>
       <c r="D25" s="13" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -18300,16 +18300,16 @@
         <v>385</v>
       </c>
       <c r="B26" s="13" t="s">
+        <v>478</v>
+      </c>
+      <c r="C26" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="D26" s="13" t="s">
         <v>480</v>
       </c>
-      <c r="D26" s="13" t="s">
-        <v>481</v>
-      </c>
       <c r="E26" s="13" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -18320,13 +18320,13 @@
         <v>447</v>
       </c>
       <c r="C27" s="13" t="s">
+        <v>529</v>
+      </c>
+      <c r="D27" s="13" t="s">
         <v>530</v>
       </c>
-      <c r="D27" s="13" t="s">
-        <v>531</v>
-      </c>
       <c r="E27" s="13" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
@@ -18334,16 +18334,16 @@
         <v>388</v>
       </c>
       <c r="B28" s="13" t="s">
+        <v>481</v>
+      </c>
+      <c r="C28" s="16" t="s">
         <v>482</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="D28" s="13" t="s">
         <v>483</v>
       </c>
-      <c r="D28" s="13" t="s">
-        <v>484</v>
-      </c>
       <c r="E28" s="13" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -18354,13 +18354,13 @@
         <v>463</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="38.4" x14ac:dyDescent="0.3">
@@ -18371,13 +18371,13 @@
         <v>20</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="112.8" x14ac:dyDescent="0.3">
@@ -18388,13 +18388,13 @@
         <v>409</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -18402,16 +18402,16 @@
         <v>415</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -18419,16 +18419,16 @@
         <v>425</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -18439,13 +18439,13 @@
         <v>301</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D34" s="21" t="s">
         <v>301</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -18465,9 +18465,9 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18478,10 +18478,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="18" customFormat="1" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
+        <v>532</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>533</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -18489,7 +18489,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -18497,7 +18497,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -18505,7 +18505,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -18513,7 +18513,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -18521,7 +18521,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -18529,7 +18529,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
@@ -18537,7 +18537,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -18545,7 +18545,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -18553,7 +18553,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -18561,7 +18561,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
   </sheetData>
@@ -18587,15 +18587,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>490</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B2" s="1">
         <v>1600</v>
@@ -18603,7 +18603,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B3" s="1">
         <v>1520</v>
@@ -18611,7 +18611,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B4" s="1">
         <v>1360</v>
@@ -18619,7 +18619,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B5" s="1">
         <v>1280</v>
@@ -18655,15 +18655,15 @@
         <v>5</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>490</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C2" t="str">
         <f>role_sen</f>
@@ -18676,7 +18676,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C3" t="str">
         <f>role_pm</f>
@@ -18770,7 +18770,7 @@
         <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C10" t="str">
         <f>role_sup</f>
@@ -18859,21 +18859,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101000E42A224B9113542A2FDED1887CD85E2" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="8844a2395c15a83707b1be2825cf9502">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e2e9d566-b848-4035-b241-3916f8cf0025" xmlns:ns3="0a6faf20-d899-469e-a43c-3306f10c465a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b26fa51f9f2fd040efc4ccb464bd5006" ns2:_="" ns3:_="">
     <xsd:import namespace="e2e9d566-b848-4035-b241-3916f8cf0025"/>
@@ -19078,24 +19063,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D022D483-5895-40DF-A800-5C8C35B62290}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA17A7A6-AB89-4C3B-8459-1F56AB738DDA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{325BCB7D-EB96-4D22-9200-77BA93C1C5DE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19112,4 +19095,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA17A7A6-AB89-4C3B-8459-1F56AB738DDA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D022D483-5895-40DF-A800-5C8C35B62290}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>